<commit_message>
annotation of new terms
</commit_message>
<xml_diff>
--- a/annotation-mappings.xlsx
+++ b/annotation-mappings.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
   <si>
     <t>Field</t>
   </si>
@@ -33,15 +33,9 @@
     <t>_id</t>
   </si>
   <si>
-    <t>partNumber</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>Name of field not appropiate maybe device name is better</t>
-  </si>
-  <si>
     <t>macAddress</t>
   </si>
   <si>
@@ -214,13 +208,25 @@
   </si>
   <si>
     <t>iot:Band</t>
+  </si>
+  <si>
+    <t>board</t>
+  </si>
+  <si>
+    <t>serialNumber</t>
+  </si>
+  <si>
+    <t> http://purl.obolibrary.org/obo/IAO_0000131</t>
+  </si>
+  <si>
+    <t>http://ns.cerise-project.nl/energy/def/cim-smartgrid/#ElectronicAddress.mac</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,6 +237,14 @@
     <font>
       <sz val="11"/>
       <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -253,15 +267,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -278,8 +295,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:D27" totalsRowShown="0">
-  <autoFilter ref="B2:D27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:D28" totalsRowShown="0">
+  <autoFilter ref="B2:D28"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Field"/>
     <tableColumn id="2" name="Semantic Notation"/>
@@ -598,17 +615,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F20"/>
+  <dimension ref="B2:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.5703125" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="47" customWidth="1"/>
   </cols>
@@ -618,13 +635,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -632,123 +649,123 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>58</v>
+        <v>62</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="1"/>
+        <v>46</v>
+      </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="1"/>
+        <v>47</v>
+      </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" t="s">
-        <v>42</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" t="s">
-        <v>61</v>
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -756,38 +773,49 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" t="s">
-        <v>47</v>
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
         <v>45</v>
-      </c>
-      <c r="C19" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" display="http://purl.obolibrary.org/obo/IAO_0000131"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -813,97 +841,97 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated vocabulary mapping excel file
</commit_message>
<xml_diff>
--- a/annotation-mappings.xlsx
+++ b/annotation-mappings.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="74">
   <si>
     <t>Field</t>
   </si>
@@ -75,9 +75,6 @@
     <t>variable</t>
   </si>
   <si>
-    <t>sensors- type</t>
-  </si>
-  <si>
     <t>variable - unit</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>vcard:Location</t>
   </si>
   <si>
-    <t>vcard:longitude</t>
-  </si>
-  <si>
     <t>StartDate</t>
   </si>
   <si>
@@ -144,9 +138,6 @@
     <t>Yellow Font: Potential, not implemented</t>
   </si>
   <si>
-    <t xml:space="preserve">vcard:latitude </t>
-  </si>
-  <si>
     <t>deprecated notation</t>
   </si>
   <si>
@@ -171,9 +162,6 @@
     <t>vcard:hasCountryName</t>
   </si>
   <si>
-    <t>vcard:hasname</t>
-  </si>
-  <si>
     <t>iot:unit</t>
   </si>
   <si>
@@ -220,6 +208,45 @@
   </si>
   <si>
     <t>http://ns.cerise-project.nl/energy/def/cim-smartgrid/#ElectronicAddress.mac</t>
+  </si>
+  <si>
+    <t>need notation for board name</t>
+  </si>
+  <si>
+    <t>datasheet</t>
+  </si>
+  <si>
+    <t>ssn:SensorDataSheet</t>
+  </si>
+  <si>
+    <t>dul:hasLocation</t>
+  </si>
+  <si>
+    <t>geo:lat</t>
+  </si>
+  <si>
+    <t>geo:long</t>
+  </si>
+  <si>
+    <t>valMin</t>
+  </si>
+  <si>
+    <t>valMax</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
+    <t>iot:maximum</t>
+  </si>
+  <si>
+    <t>iot:minimum</t>
+  </si>
+  <si>
+    <t>ssn:Frequency</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
 </sst>
 </file>
@@ -250,12 +277,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -271,11 +304,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -295,8 +329,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:D28" totalsRowShown="0">
-  <autoFilter ref="B2:D28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:D29" totalsRowShown="0">
+  <autoFilter ref="B2:D29"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Field"/>
     <tableColumn id="2" name="Semantic Notation"/>
@@ -615,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F21"/>
+  <dimension ref="B2:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,13 +669,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -649,34 +683,38 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
         <v>61</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="B5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" t="s">
-        <v>56</v>
+      <c r="C6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -684,128 +722,160 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="1"/>
+        <v>63</v>
+      </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="1"/>
+        <v>43</v>
+      </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="1"/>
+        <v>44</v>
+      </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" t="s">
-        <v>40</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>66</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" t="s">
-        <v>59</v>
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" t="s">
-        <v>45</v>
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -841,7 +911,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
@@ -849,89 +919,89 @@
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" t="s">
         <v>50</v>
-      </c>
-      <c r="D9" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Development version of the SCLLV
</commit_message>
<xml_diff>
--- a/annotation-mappings.xlsx
+++ b/annotation-mappings.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="device.json" sheetId="1" r:id="rId1"/>
-    <sheet name="weekdataset.json" sheetId="2" r:id="rId2"/>
+    <sheet name="SCLL Vocabulary" sheetId="3" r:id="rId2"/>
+    <sheet name="weekdataset.json" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="155">
   <si>
     <t>Field</t>
   </si>
@@ -247,13 +248,444 @@
   </si>
   <si>
     <t>type</t>
+  </si>
+  <si>
+    <t>Namespaces</t>
+  </si>
+  <si>
+    <t>Context Definitions</t>
+  </si>
+  <si>
+    <t>Extended Vocabulary</t>
+  </si>
+  <si>
+    <t>"xsd" : "http://www.w3.org/2001/XMLSchema#"</t>
+  </si>
+  <si>
+    <t>"rdfs": "http://www.w3.org/2000/01/rdf-schema#"</t>
+  </si>
+  <si>
+    <t>"ssn" : "http://purl.oclc.org/NET/ssnx/ssn#"</t>
+  </si>
+  <si>
+    <t>"vcard": "http://www.w3.org/2006/vcard/ns#"</t>
+  </si>
+  <si>
+    <t>"iot": "https://iotdb.org/pub/iot#"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "dc" : "http://purl.org/dc/elements/1.1/"</t>
+  </si>
+  <si>
+    <t>"dul" : "http://www.loa-cnr.it/ontologies/DUL.owl#"</t>
+  </si>
+  <si>
+    <t>"geo" : "http://www.w3.org/2003/01/geo/wgs84_pos#"</t>
+  </si>
+  <si>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>dc:date</t>
+  </si>
+  <si>
+    <t>rdfs:label</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>rdfs:comment</t>
+  </si>
+  <si>
+    <t>xsd:string</t>
+  </si>
+  <si>
+    <t>iot:Unit</t>
+  </si>
+  <si>
+    <t>"iot-unit": "https://iotdb.org/pub/iot-unit#"</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>vocab</t>
+  </si>
+  <si>
+    <t>http://ontology.cybershare.utep.edu/livinglab/ssll.jsonld</t>
+  </si>
+  <si>
+    <t>http://ontology.cybershare.utep.edu/livinglab/sll#</t>
+  </si>
+  <si>
+    <t>http://ontology.cybershare.utep.edu/livinglab/ssll</t>
+  </si>
+  <si>
+    <t>versionInfo</t>
+  </si>
+  <si>
+    <t>owl:versionInfo</t>
+  </si>
+  <si>
+    <t>Smart Cities Living Lab Vocabulary</t>
+  </si>
+  <si>
+    <t>#temperature</t>
+  </si>
+  <si>
+    <t>#pressure</t>
+  </si>
+  <si>
+    <t>#noise</t>
+  </si>
+  <si>
+    <t>#light</t>
+  </si>
+  <si>
+    <t>additional attributes</t>
+  </si>
+  <si>
+    <t>iot:Attribute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"iot:purpose": "iot-purpose:temperature",
+"iot:unit": "iot-unit:temperature.si.celsius",
+"iot:type": "iot:type.number", "iot:read": true,
+"iot:write": false,
+"iot:sensor": true,
+"iot:actuator": false
+</t>
+  </si>
+  <si>
+    <t>numeric pressure value measured un Kilo Pascal by a barometer sensor</t>
+  </si>
+  <si>
+    <t>numeric temperature value measured in celsius by a temperature sensor</t>
+  </si>
+  <si>
+    <t>numeric noise value measured in decibels by a microphone sensor</t>
+  </si>
+  <si>
+    <t>numeric light value measured in lumens by a light sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "iot:purpose": "iot-purpose:pressure",
+      "iot:unit": "iot-unit:pressure.si.pascal.3",
+      "iot:type": "iot:type.number",
+      "iot:read": true,
+      "iot:write": false,
+      "iot:sensor": true,
+      "iot:actuator": false
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "iot:purpose": "iot-purpose:sound",
+      "iot:unit": "iot-unit:math.fraction.percent",
+      "iot:type": "iot:type.number",
+      "iot:read": true,
+      "iot:write": false,
+      "iot:sensor": true,
+      "iot:actuator": false
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "iot:purpose": "iot-purpose:light",
+      "iot:unit": "iot-unit:math.fraction.percent",
+      "iot:type": "iot:type.number",
+      "iot:read": true,
+      "iot:write": false,
+      "iot:sensor": true,
+      "iot:actuator": false
+</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>rdfs:range</t>
+  </si>
+  <si>
+    <t>xsd:double</t>
+  </si>
+  <si>
+    <t>xsd:integer</t>
+  </si>
+  <si>
+    <t>xsd:anyURI</t>
+  </si>
+  <si>
+    <t>xsd:float</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "prov" : "http://www.w3.org/ns/prov#"</t>
+  </si>
+  <si>
+    <r>
+      <t>"owl"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA71D5D"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF183691"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"http://www.w3.org/2002/07/owl#"</t>
+    </r>
+  </si>
+  <si>
+    <t>xsd:dateTime</t>
+  </si>
+  <si>
+    <t>Observation Extension</t>
+  </si>
+  <si>
+    <t>Custom extended vocabulary for the UDG Smart Cities Living Lab  Sensor Network</t>
+  </si>
+  <si>
+    <t>#board</t>
+  </si>
+  <si>
+    <t>#serialNumber</t>
+  </si>
+  <si>
+    <t>#macAddress</t>
+  </si>
+  <si>
+    <t>#protocol</t>
+  </si>
+  <si>
+    <t>#partName</t>
+  </si>
+  <si>
+    <t>#sensor (change to characteristic)</t>
+  </si>
+  <si>
+    <t>#type</t>
+  </si>
+  <si>
+    <t>serial number</t>
+  </si>
+  <si>
+    <t>mac address</t>
+  </si>
+  <si>
+    <t>part name</t>
+  </si>
+  <si>
+    <t>sensor</t>
+  </si>
+  <si>
+    <t>measurement</t>
+  </si>
+  <si>
+    <t>#measurement (change to entity)</t>
+  </si>
+  <si>
+    <t>owl:Class</t>
+  </si>
+  <si>
+    <t>owl:DatatypeProperty</t>
+  </si>
+  <si>
+    <t>development prototyping board based on microcontroller architectures</t>
+  </si>
+  <si>
+    <t> a unique identifier assigned incrementally or sequentially to an item</t>
+  </si>
+  <si>
+    <r>
+      <t>A </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF252525"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>media access control address</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF252525"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF252525"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>MAC address</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF252525"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>), also called a physical address, of a computer which is a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>unique identifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF252525"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> assigned to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>network interfaces</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF252525"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> for communications on the physical network segment.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>is a system of rules that allow two or more entities of a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>communications system</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF252525"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> to transmit </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>information</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF252525"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> via any kind of variation of a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>physical quantity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF252525"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>. </t>
+    </r>
+  </si>
+  <si>
+    <t>a word that names a part of a larger whole</t>
+  </si>
+  <si>
+    <t>an environmental characteristic</t>
+  </si>
+  <si>
+    <t>digital or analalog</t>
+  </si>
+  <si>
+    <t>an entity…..</t>
+  </si>
+  <si>
+    <t>Metadata Extension (posible ontology)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,6 +707,49 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF183691"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFA71D5D"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF252525"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0B0080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF252525"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF404040"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -304,12 +779,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -651,7 +1135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -891,6 +1375,663 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="63.42578125" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="74.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>103</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>120</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>29</v>
+      </c>
+      <c r="B46" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51" t="s">
+        <v>87</v>
+      </c>
+      <c r="D51" t="s">
+        <v>88</v>
+      </c>
+      <c r="E51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>105</v>
+      </c>
+      <c r="D52" t="s">
+        <v>130</v>
+      </c>
+      <c r="E52">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>86</v>
+      </c>
+      <c r="B56" t="s">
+        <v>73</v>
+      </c>
+      <c r="C56" t="s">
+        <v>87</v>
+      </c>
+      <c r="D56" t="s">
+        <v>88</v>
+      </c>
+      <c r="E56" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="181.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>106</v>
+      </c>
+      <c r="B57" t="s">
+        <v>111</v>
+      </c>
+      <c r="C57" t="s">
+        <v>28</v>
+      </c>
+      <c r="D57" t="s">
+        <v>114</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>107</v>
+      </c>
+      <c r="B58" t="s">
+        <v>111</v>
+      </c>
+      <c r="C58" t="s">
+        <v>24</v>
+      </c>
+      <c r="D58" t="s">
+        <v>113</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>108</v>
+      </c>
+      <c r="B59" t="s">
+        <v>111</v>
+      </c>
+      <c r="C59" t="s">
+        <v>27</v>
+      </c>
+      <c r="D59" t="s">
+        <v>115</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>109</v>
+      </c>
+      <c r="B60" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" t="s">
+        <v>26</v>
+      </c>
+      <c r="D60" t="s">
+        <v>116</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>131</v>
+      </c>
+      <c r="B64" t="s">
+        <v>144</v>
+      </c>
+      <c r="C64" t="s">
+        <v>57</v>
+      </c>
+      <c r="D64" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>132</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C65" t="s">
+        <v>138</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="39" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>133</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C66" t="s">
+        <v>139</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>134</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C67" t="s">
+        <v>4</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>135</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C68" t="s">
+        <v>140</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C69" t="s">
+        <v>141</v>
+      </c>
+      <c r="D69" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>137</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C70" t="s">
+        <v>73</v>
+      </c>
+      <c r="D70" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>143</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C71" t="s">
+        <v>142</v>
+      </c>
+      <c r="D71" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A18" r:id="rId1"/>
+    <hyperlink ref="B16" r:id="rId2"/>
+    <hyperlink ref="A54" r:id="rId3"/>
+    <hyperlink ref="D65" r:id="rId4" tooltip="Unique identifier" display="https://en.wikipedia.org/wiki/Unique_identifier"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D12"/>
   <sheetViews>

</xml_diff>